<commit_message>
Eliminación de tildes y ñ's para el correcto funcionamiento de Linux
</commit_message>
<xml_diff>
--- a/data/Elementos.xlsx
+++ b/data/Elementos.xlsx
@@ -5,7 +5,7 @@
   <workbookPr defaultThemeVersion="164011"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\TFG\Codigo\ProyectoFinal\XpectraJ\build\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Pablo\Desktop\TFG\Codigo\ProyectoFinal\XpectraC\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
@@ -21,9 +21,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="118">
   <si>
-    <t>Hidrógeno</t>
-  </si>
-  <si>
     <t>Helio</t>
   </si>
   <si>
@@ -39,18 +36,6 @@
     <t>Carbono</t>
   </si>
   <si>
-    <t>Nitrógeno</t>
-  </si>
-  <si>
-    <t>Oxígeno</t>
-  </si>
-  <si>
-    <t>Flúor</t>
-  </si>
-  <si>
-    <t>Neón</t>
-  </si>
-  <si>
     <t>Sodio</t>
   </si>
   <si>
@@ -63,18 +48,12 @@
     <t>Silicio</t>
   </si>
   <si>
-    <t>Fósforo</t>
-  </si>
-  <si>
     <t>Azufre</t>
   </si>
   <si>
     <t>Cloro</t>
   </si>
   <si>
-    <t>Argón</t>
-  </si>
-  <si>
     <t>Potasio</t>
   </si>
   <si>
@@ -126,9 +105,6 @@
     <t>Bromo</t>
   </si>
   <si>
-    <t>Kriptón</t>
-  </si>
-  <si>
     <t>Rubidio</t>
   </si>
   <si>
@@ -168,9 +144,6 @@
     <t>Indio</t>
   </si>
   <si>
-    <t>Estaño</t>
-  </si>
-  <si>
     <t>Antimonio</t>
   </si>
   <si>
@@ -180,9 +153,6 @@
     <t>Yodo</t>
   </si>
   <si>
-    <t>Xenón</t>
-  </si>
-  <si>
     <t>Cesio</t>
   </si>
   <si>
@@ -237,9 +207,6 @@
     <t>Hafnio</t>
   </si>
   <si>
-    <t>Tántalo</t>
-  </si>
-  <si>
     <t>Wolframio</t>
   </si>
   <si>
@@ -276,9 +243,6 @@
     <t>Astato</t>
   </si>
   <si>
-    <t>Radón</t>
-  </si>
-  <si>
     <t>Francio</t>
   </si>
   <si>
@@ -373,6 +337,42 @@
   </si>
   <si>
     <t>Ununoctio</t>
+  </si>
+  <si>
+    <t>HidrOgeno</t>
+  </si>
+  <si>
+    <t>NitrOgeno</t>
+  </si>
+  <si>
+    <t>OxIgeno</t>
+  </si>
+  <si>
+    <t>FlUor</t>
+  </si>
+  <si>
+    <t>NeOn</t>
+  </si>
+  <si>
+    <t>FOsforo</t>
+  </si>
+  <si>
+    <t>ArgOn</t>
+  </si>
+  <si>
+    <t>KriptOn</t>
+  </si>
+  <si>
+    <t>EstaNo</t>
+  </si>
+  <si>
+    <t>XenOn</t>
+  </si>
+  <si>
+    <t>TAntalo</t>
+  </si>
+  <si>
+    <t>RadOn</t>
   </si>
 </sst>
 </file>
@@ -1215,7 +1215,9 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
+      <selection activeCell="B119" sqref="B119"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
@@ -1224,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>0</v>
+        <v>106</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1232,7 +1234,7 @@
         <v>2</v>
       </c>
       <c r="B2" t="s">
-        <v>1</v>
+        <v>0</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.3">
@@ -1240,7 +1242,7 @@
         <v>3</v>
       </c>
       <c r="B3" t="s">
-        <v>2</v>
+        <v>1</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.3">
@@ -1248,7 +1250,7 @@
         <v>4</v>
       </c>
       <c r="B4" t="s">
-        <v>3</v>
+        <v>2</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.3">
@@ -1256,7 +1258,7 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.3">
@@ -1264,7 +1266,7 @@
         <v>6</v>
       </c>
       <c r="B6" t="s">
-        <v>5</v>
+        <v>4</v>
       </c>
     </row>
     <row r="7" spans="1:2" x14ac:dyDescent="0.3">
@@ -1272,7 +1274,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>6</v>
+        <v>107</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1280,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>7</v>
+        <v>108</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1288,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>8</v>
+        <v>109</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1296,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>9</v>
+        <v>110</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1304,7 +1306,7 @@
         <v>11</v>
       </c>
       <c r="B11" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
     </row>
     <row r="12" spans="1:2" x14ac:dyDescent="0.3">
@@ -1312,7 +1314,7 @@
         <v>12</v>
       </c>
       <c r="B12" t="s">
-        <v>11</v>
+        <v>6</v>
       </c>
     </row>
     <row r="13" spans="1:2" x14ac:dyDescent="0.3">
@@ -1320,7 +1322,7 @@
         <v>13</v>
       </c>
       <c r="B13" t="s">
-        <v>12</v>
+        <v>7</v>
       </c>
     </row>
     <row r="14" spans="1:2" x14ac:dyDescent="0.3">
@@ -1328,7 +1330,7 @@
         <v>14</v>
       </c>
       <c r="B14" t="s">
-        <v>13</v>
+        <v>8</v>
       </c>
     </row>
     <row r="15" spans="1:2" x14ac:dyDescent="0.3">
@@ -1336,7 +1338,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>14</v>
+        <v>111</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1344,7 +1346,7 @@
         <v>16</v>
       </c>
       <c r="B16" t="s">
-        <v>15</v>
+        <v>9</v>
       </c>
     </row>
     <row r="17" spans="1:2" x14ac:dyDescent="0.3">
@@ -1352,7 +1354,7 @@
         <v>17</v>
       </c>
       <c r="B17" t="s">
-        <v>16</v>
+        <v>10</v>
       </c>
     </row>
     <row r="18" spans="1:2" x14ac:dyDescent="0.3">
@@ -1360,7 +1362,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>17</v>
+        <v>112</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1368,7 +1370,7 @@
         <v>19</v>
       </c>
       <c r="B19" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.3">
@@ -1376,7 +1378,7 @@
         <v>20</v>
       </c>
       <c r="B20" t="s">
-        <v>19</v>
+        <v>12</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.3">
@@ -1384,7 +1386,7 @@
         <v>21</v>
       </c>
       <c r="B21" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
     <row r="22" spans="1:2" x14ac:dyDescent="0.3">
@@ -1392,7 +1394,7 @@
         <v>22</v>
       </c>
       <c r="B22" t="s">
-        <v>21</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.3">
@@ -1400,7 +1402,7 @@
         <v>23</v>
       </c>
       <c r="B23" t="s">
-        <v>22</v>
+        <v>15</v>
       </c>
     </row>
     <row r="24" spans="1:2" x14ac:dyDescent="0.3">
@@ -1408,7 +1410,7 @@
         <v>24</v>
       </c>
       <c r="B24" t="s">
-        <v>23</v>
+        <v>16</v>
       </c>
     </row>
     <row r="25" spans="1:2" x14ac:dyDescent="0.3">
@@ -1416,7 +1418,7 @@
         <v>25</v>
       </c>
       <c r="B25" t="s">
-        <v>24</v>
+        <v>17</v>
       </c>
     </row>
     <row r="26" spans="1:2" x14ac:dyDescent="0.3">
@@ -1424,7 +1426,7 @@
         <v>26</v>
       </c>
       <c r="B26" t="s">
-        <v>25</v>
+        <v>18</v>
       </c>
     </row>
     <row r="27" spans="1:2" x14ac:dyDescent="0.3">
@@ -1432,7 +1434,7 @@
         <v>27</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>19</v>
       </c>
     </row>
     <row r="28" spans="1:2" x14ac:dyDescent="0.3">
@@ -1440,7 +1442,7 @@
         <v>28</v>
       </c>
       <c r="B28" t="s">
-        <v>27</v>
+        <v>20</v>
       </c>
     </row>
     <row r="29" spans="1:2" x14ac:dyDescent="0.3">
@@ -1448,7 +1450,7 @@
         <v>29</v>
       </c>
       <c r="B29" t="s">
-        <v>28</v>
+        <v>21</v>
       </c>
     </row>
     <row r="30" spans="1:2" x14ac:dyDescent="0.3">
@@ -1456,7 +1458,7 @@
         <v>30</v>
       </c>
       <c r="B30" t="s">
-        <v>29</v>
+        <v>22</v>
       </c>
     </row>
     <row r="31" spans="1:2" x14ac:dyDescent="0.3">
@@ -1464,7 +1466,7 @@
         <v>31</v>
       </c>
       <c r="B31" t="s">
-        <v>30</v>
+        <v>23</v>
       </c>
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.3">
@@ -1472,7 +1474,7 @@
         <v>32</v>
       </c>
       <c r="B32" t="s">
-        <v>31</v>
+        <v>24</v>
       </c>
     </row>
     <row r="33" spans="1:2" x14ac:dyDescent="0.3">
@@ -1480,7 +1482,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>32</v>
+        <v>25</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1488,7 +1490,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>33</v>
+        <v>26</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1496,7 +1498,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>34</v>
+        <v>27</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1504,7 +1506,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>35</v>
+        <v>113</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1512,7 +1514,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>36</v>
+        <v>28</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1520,7 +1522,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>37</v>
+        <v>29</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1528,7 +1530,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>38</v>
+        <v>30</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1536,7 +1538,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>39</v>
+        <v>31</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1544,7 +1546,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>40</v>
+        <v>32</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1552,7 +1554,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>41</v>
+        <v>33</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1560,7 +1562,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>42</v>
+        <v>34</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1568,7 +1570,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>43</v>
+        <v>35</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1576,7 +1578,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1584,7 +1586,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>45</v>
+        <v>37</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1592,7 +1594,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>46</v>
+        <v>38</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1600,7 +1602,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>47</v>
+        <v>39</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1608,7 +1610,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>48</v>
+        <v>40</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1616,7 +1618,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>49</v>
+        <v>114</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1624,7 +1626,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>50</v>
+        <v>41</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1632,7 +1634,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>51</v>
+        <v>42</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1640,7 +1642,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>52</v>
+        <v>43</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1648,7 +1650,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>53</v>
+        <v>115</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1656,7 +1658,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>54</v>
+        <v>44</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1664,7 +1666,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>55</v>
+        <v>45</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1672,7 +1674,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>56</v>
+        <v>46</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1680,7 +1682,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>57</v>
+        <v>47</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1688,7 +1690,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>58</v>
+        <v>48</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1696,7 +1698,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>59</v>
+        <v>49</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1704,7 +1706,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>60</v>
+        <v>50</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1712,7 +1714,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>61</v>
+        <v>51</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1720,7 +1722,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>62</v>
+        <v>52</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1728,7 +1730,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>63</v>
+        <v>53</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1736,7 +1738,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>64</v>
+        <v>54</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1744,7 +1746,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>65</v>
+        <v>55</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1752,7 +1754,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>66</v>
+        <v>56</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1760,7 +1762,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>67</v>
+        <v>57</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1768,7 +1770,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>68</v>
+        <v>58</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1776,7 +1778,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>69</v>
+        <v>59</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1784,7 +1786,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>70</v>
+        <v>60</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1792,7 +1794,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>71</v>
+        <v>61</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1800,7 +1802,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>72</v>
+        <v>116</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1808,7 +1810,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>73</v>
+        <v>62</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1816,7 +1818,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>74</v>
+        <v>63</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1824,7 +1826,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>75</v>
+        <v>64</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1832,7 +1834,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>76</v>
+        <v>65</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1840,7 +1842,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>77</v>
+        <v>66</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1848,7 +1850,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>78</v>
+        <v>67</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1856,7 +1858,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>79</v>
+        <v>68</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1864,7 +1866,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>80</v>
+        <v>69</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1872,7 +1874,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>81</v>
+        <v>70</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1880,7 +1882,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>82</v>
+        <v>71</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1888,7 +1890,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>83</v>
+        <v>72</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1896,7 +1898,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>84</v>
+        <v>73</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1904,7 +1906,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>85</v>
+        <v>117</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1912,7 +1914,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>86</v>
+        <v>74</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1920,7 +1922,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>87</v>
+        <v>75</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1928,7 +1930,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1936,7 +1938,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>89</v>
+        <v>77</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1944,7 +1946,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>90</v>
+        <v>78</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1952,7 +1954,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>91</v>
+        <v>79</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1960,7 +1962,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>92</v>
+        <v>80</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1968,7 +1970,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>93</v>
+        <v>81</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1976,7 +1978,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>94</v>
+        <v>82</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1984,7 +1986,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>95</v>
+        <v>83</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1992,7 +1994,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>96</v>
+        <v>84</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -2000,7 +2002,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>97</v>
+        <v>85</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2008,7 +2010,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>98</v>
+        <v>86</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2016,7 +2018,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>99</v>
+        <v>87</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2024,7 +2026,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>100</v>
+        <v>88</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2032,7 +2034,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>101</v>
+        <v>89</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2040,7 +2042,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>102</v>
+        <v>90</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2048,7 +2050,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>103</v>
+        <v>91</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -2056,7 +2058,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>104</v>
+        <v>92</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2064,7 +2066,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>105</v>
+        <v>93</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2072,7 +2074,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>106</v>
+        <v>94</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2080,7 +2082,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>107</v>
+        <v>95</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2088,7 +2090,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>108</v>
+        <v>96</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -2096,7 +2098,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>109</v>
+        <v>97</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -2104,7 +2106,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>110</v>
+        <v>98</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2112,7 +2114,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>111</v>
+        <v>99</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -2120,7 +2122,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2128,7 +2130,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>113</v>
+        <v>101</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -2136,7 +2138,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>114</v>
+        <v>102</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -2144,7 +2146,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>115</v>
+        <v>103</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -2152,7 +2154,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>116</v>
+        <v>104</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -2160,7 +2162,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>117</v>
+        <v>105</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Corrección tildes y ñ's para buen funcionamiento en Linux
</commit_message>
<xml_diff>
--- a/data/Elementos.xlsx
+++ b/data/Elementos.xlsx
@@ -96,9 +96,6 @@
     <t>Germanio</t>
   </si>
   <si>
-    <t>Arsénico</t>
-  </si>
-  <si>
     <t>Selenio</t>
   </si>
   <si>
@@ -373,6 +370,9 @@
   </si>
   <si>
     <t>RadOn</t>
+  </si>
+  <si>
+    <t>ArsEnico</t>
   </si>
 </sst>
 </file>
@@ -1215,8 +1215,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B118"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A103" workbookViewId="0">
-      <selection activeCell="B119" sqref="B119"/>
+    <sheetView tabSelected="1" topLeftCell="A105" workbookViewId="0">
+      <selection activeCell="B121" sqref="B121"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1226,7 +1226,7 @@
         <v>1</v>
       </c>
       <c r="B1" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
     </row>
     <row r="2" spans="1:2" x14ac:dyDescent="0.3">
@@ -1274,7 +1274,7 @@
         <v>7</v>
       </c>
       <c r="B7" t="s">
-        <v>107</v>
+        <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.3">
@@ -1282,7 +1282,7 @@
         <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>108</v>
+        <v>107</v>
       </c>
     </row>
     <row r="9" spans="1:2" x14ac:dyDescent="0.3">
@@ -1290,7 +1290,7 @@
         <v>9</v>
       </c>
       <c r="B9" t="s">
-        <v>109</v>
+        <v>108</v>
       </c>
     </row>
     <row r="10" spans="1:2" x14ac:dyDescent="0.3">
@@ -1298,7 +1298,7 @@
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>110</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.3">
@@ -1338,7 +1338,7 @@
         <v>15</v>
       </c>
       <c r="B15" t="s">
-        <v>111</v>
+        <v>110</v>
       </c>
     </row>
     <row r="16" spans="1:2" x14ac:dyDescent="0.3">
@@ -1362,7 +1362,7 @@
         <v>18</v>
       </c>
       <c r="B18" t="s">
-        <v>112</v>
+        <v>111</v>
       </c>
     </row>
     <row r="19" spans="1:2" x14ac:dyDescent="0.3">
@@ -1482,7 +1482,7 @@
         <v>33</v>
       </c>
       <c r="B33" t="s">
-        <v>25</v>
+        <v>117</v>
       </c>
     </row>
     <row r="34" spans="1:2" x14ac:dyDescent="0.3">
@@ -1490,7 +1490,7 @@
         <v>34</v>
       </c>
       <c r="B34" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.3">
@@ -1498,7 +1498,7 @@
         <v>35</v>
       </c>
       <c r="B35" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
     </row>
     <row r="36" spans="1:2" x14ac:dyDescent="0.3">
@@ -1506,7 +1506,7 @@
         <v>36</v>
       </c>
       <c r="B36" t="s">
-        <v>113</v>
+        <v>112</v>
       </c>
     </row>
     <row r="37" spans="1:2" x14ac:dyDescent="0.3">
@@ -1514,7 +1514,7 @@
         <v>37</v>
       </c>
       <c r="B37" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
     </row>
     <row r="38" spans="1:2" x14ac:dyDescent="0.3">
@@ -1522,7 +1522,7 @@
         <v>38</v>
       </c>
       <c r="B38" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
     </row>
     <row r="39" spans="1:2" x14ac:dyDescent="0.3">
@@ -1530,7 +1530,7 @@
         <v>39</v>
       </c>
       <c r="B39" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
     </row>
     <row r="40" spans="1:2" x14ac:dyDescent="0.3">
@@ -1538,7 +1538,7 @@
         <v>40</v>
       </c>
       <c r="B40" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
     </row>
     <row r="41" spans="1:2" x14ac:dyDescent="0.3">
@@ -1546,7 +1546,7 @@
         <v>41</v>
       </c>
       <c r="B41" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
     </row>
     <row r="42" spans="1:2" x14ac:dyDescent="0.3">
@@ -1554,7 +1554,7 @@
         <v>42</v>
       </c>
       <c r="B42" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
     </row>
     <row r="43" spans="1:2" x14ac:dyDescent="0.3">
@@ -1562,7 +1562,7 @@
         <v>43</v>
       </c>
       <c r="B43" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
     </row>
     <row r="44" spans="1:2" x14ac:dyDescent="0.3">
@@ -1570,7 +1570,7 @@
         <v>44</v>
       </c>
       <c r="B44" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
     </row>
     <row r="45" spans="1:2" x14ac:dyDescent="0.3">
@@ -1578,7 +1578,7 @@
         <v>45</v>
       </c>
       <c r="B45" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
     </row>
     <row r="46" spans="1:2" x14ac:dyDescent="0.3">
@@ -1586,7 +1586,7 @@
         <v>46</v>
       </c>
       <c r="B46" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
     </row>
     <row r="47" spans="1:2" x14ac:dyDescent="0.3">
@@ -1594,7 +1594,7 @@
         <v>47</v>
       </c>
       <c r="B47" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
     </row>
     <row r="48" spans="1:2" x14ac:dyDescent="0.3">
@@ -1602,7 +1602,7 @@
         <v>48</v>
       </c>
       <c r="B48" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
     </row>
     <row r="49" spans="1:2" x14ac:dyDescent="0.3">
@@ -1610,7 +1610,7 @@
         <v>49</v>
       </c>
       <c r="B49" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
     </row>
     <row r="50" spans="1:2" x14ac:dyDescent="0.3">
@@ -1618,7 +1618,7 @@
         <v>50</v>
       </c>
       <c r="B50" t="s">
-        <v>114</v>
+        <v>113</v>
       </c>
     </row>
     <row r="51" spans="1:2" x14ac:dyDescent="0.3">
@@ -1626,7 +1626,7 @@
         <v>51</v>
       </c>
       <c r="B51" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
     </row>
     <row r="52" spans="1:2" x14ac:dyDescent="0.3">
@@ -1634,7 +1634,7 @@
         <v>52</v>
       </c>
       <c r="B52" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
     </row>
     <row r="53" spans="1:2" x14ac:dyDescent="0.3">
@@ -1642,7 +1642,7 @@
         <v>53</v>
       </c>
       <c r="B53" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
     </row>
     <row r="54" spans="1:2" x14ac:dyDescent="0.3">
@@ -1650,7 +1650,7 @@
         <v>54</v>
       </c>
       <c r="B54" t="s">
-        <v>115</v>
+        <v>114</v>
       </c>
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
@@ -1658,7 +1658,7 @@
         <v>55</v>
       </c>
       <c r="B55" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
@@ -1666,7 +1666,7 @@
         <v>56</v>
       </c>
       <c r="B56" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="57" spans="1:2" x14ac:dyDescent="0.3">
@@ -1674,7 +1674,7 @@
         <v>57</v>
       </c>
       <c r="B57" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="58" spans="1:2" x14ac:dyDescent="0.3">
@@ -1682,7 +1682,7 @@
         <v>58</v>
       </c>
       <c r="B58" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="59" spans="1:2" x14ac:dyDescent="0.3">
@@ -1690,7 +1690,7 @@
         <v>59</v>
       </c>
       <c r="B59" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
     </row>
     <row r="60" spans="1:2" x14ac:dyDescent="0.3">
@@ -1698,7 +1698,7 @@
         <v>60</v>
       </c>
       <c r="B60" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
     </row>
     <row r="61" spans="1:2" x14ac:dyDescent="0.3">
@@ -1706,7 +1706,7 @@
         <v>61</v>
       </c>
       <c r="B61" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
     </row>
     <row r="62" spans="1:2" x14ac:dyDescent="0.3">
@@ -1714,7 +1714,7 @@
         <v>62</v>
       </c>
       <c r="B62" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
     </row>
     <row r="63" spans="1:2" x14ac:dyDescent="0.3">
@@ -1722,7 +1722,7 @@
         <v>63</v>
       </c>
       <c r="B63" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
     </row>
     <row r="64" spans="1:2" x14ac:dyDescent="0.3">
@@ -1730,7 +1730,7 @@
         <v>64</v>
       </c>
       <c r="B64" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
     </row>
     <row r="65" spans="1:2" x14ac:dyDescent="0.3">
@@ -1738,7 +1738,7 @@
         <v>65</v>
       </c>
       <c r="B65" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
     </row>
     <row r="66" spans="1:2" x14ac:dyDescent="0.3">
@@ -1746,7 +1746,7 @@
         <v>66</v>
       </c>
       <c r="B66" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
     </row>
     <row r="67" spans="1:2" x14ac:dyDescent="0.3">
@@ -1754,7 +1754,7 @@
         <v>67</v>
       </c>
       <c r="B67" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
     </row>
     <row r="68" spans="1:2" x14ac:dyDescent="0.3">
@@ -1762,7 +1762,7 @@
         <v>68</v>
       </c>
       <c r="B68" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
     </row>
     <row r="69" spans="1:2" x14ac:dyDescent="0.3">
@@ -1770,7 +1770,7 @@
         <v>69</v>
       </c>
       <c r="B69" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
     </row>
     <row r="70" spans="1:2" x14ac:dyDescent="0.3">
@@ -1778,7 +1778,7 @@
         <v>70</v>
       </c>
       <c r="B70" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
     </row>
     <row r="71" spans="1:2" x14ac:dyDescent="0.3">
@@ -1786,7 +1786,7 @@
         <v>71</v>
       </c>
       <c r="B71" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="72" spans="1:2" x14ac:dyDescent="0.3">
@@ -1794,7 +1794,7 @@
         <v>72</v>
       </c>
       <c r="B72" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="73" spans="1:2" x14ac:dyDescent="0.3">
@@ -1802,7 +1802,7 @@
         <v>73</v>
       </c>
       <c r="B73" t="s">
-        <v>116</v>
+        <v>115</v>
       </c>
     </row>
     <row r="74" spans="1:2" x14ac:dyDescent="0.3">
@@ -1810,7 +1810,7 @@
         <v>74</v>
       </c>
       <c r="B74" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
     <row r="75" spans="1:2" x14ac:dyDescent="0.3">
@@ -1818,7 +1818,7 @@
         <v>75</v>
       </c>
       <c r="B75" t="s">
-        <v>63</v>
+        <v>62</v>
       </c>
     </row>
     <row r="76" spans="1:2" x14ac:dyDescent="0.3">
@@ -1826,7 +1826,7 @@
         <v>76</v>
       </c>
       <c r="B76" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
     </row>
     <row r="77" spans="1:2" x14ac:dyDescent="0.3">
@@ -1834,7 +1834,7 @@
         <v>77</v>
       </c>
       <c r="B77" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
     </row>
     <row r="78" spans="1:2" x14ac:dyDescent="0.3">
@@ -1842,7 +1842,7 @@
         <v>78</v>
       </c>
       <c r="B78" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
     </row>
     <row r="79" spans="1:2" x14ac:dyDescent="0.3">
@@ -1850,7 +1850,7 @@
         <v>79</v>
       </c>
       <c r="B79" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
     </row>
     <row r="80" spans="1:2" x14ac:dyDescent="0.3">
@@ -1858,7 +1858,7 @@
         <v>80</v>
       </c>
       <c r="B80" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
     </row>
     <row r="81" spans="1:2" x14ac:dyDescent="0.3">
@@ -1866,7 +1866,7 @@
         <v>81</v>
       </c>
       <c r="B81" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
     </row>
     <row r="82" spans="1:2" x14ac:dyDescent="0.3">
@@ -1874,7 +1874,7 @@
         <v>82</v>
       </c>
       <c r="B82" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
     </row>
     <row r="83" spans="1:2" x14ac:dyDescent="0.3">
@@ -1882,7 +1882,7 @@
         <v>83</v>
       </c>
       <c r="B83" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
     </row>
     <row r="84" spans="1:2" x14ac:dyDescent="0.3">
@@ -1890,7 +1890,7 @@
         <v>84</v>
       </c>
       <c r="B84" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
     </row>
     <row r="85" spans="1:2" x14ac:dyDescent="0.3">
@@ -1898,7 +1898,7 @@
         <v>85</v>
       </c>
       <c r="B85" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
     </row>
     <row r="86" spans="1:2" x14ac:dyDescent="0.3">
@@ -1906,7 +1906,7 @@
         <v>86</v>
       </c>
       <c r="B86" t="s">
-        <v>117</v>
+        <v>116</v>
       </c>
     </row>
     <row r="87" spans="1:2" x14ac:dyDescent="0.3">
@@ -1914,7 +1914,7 @@
         <v>87</v>
       </c>
       <c r="B87" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
     </row>
     <row r="88" spans="1:2" x14ac:dyDescent="0.3">
@@ -1922,7 +1922,7 @@
         <v>88</v>
       </c>
       <c r="B88" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
     </row>
     <row r="89" spans="1:2" x14ac:dyDescent="0.3">
@@ -1930,7 +1930,7 @@
         <v>89</v>
       </c>
       <c r="B89" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
     </row>
     <row r="90" spans="1:2" x14ac:dyDescent="0.3">
@@ -1938,7 +1938,7 @@
         <v>90</v>
       </c>
       <c r="B90" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="91" spans="1:2" x14ac:dyDescent="0.3">
@@ -1946,7 +1946,7 @@
         <v>91</v>
       </c>
       <c r="B91" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="92" spans="1:2" x14ac:dyDescent="0.3">
@@ -1954,7 +1954,7 @@
         <v>92</v>
       </c>
       <c r="B92" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
     </row>
     <row r="93" spans="1:2" x14ac:dyDescent="0.3">
@@ -1962,7 +1962,7 @@
         <v>93</v>
       </c>
       <c r="B93" t="s">
-        <v>80</v>
+        <v>79</v>
       </c>
     </row>
     <row r="94" spans="1:2" x14ac:dyDescent="0.3">
@@ -1970,7 +1970,7 @@
         <v>94</v>
       </c>
       <c r="B94" t="s">
-        <v>81</v>
+        <v>80</v>
       </c>
     </row>
     <row r="95" spans="1:2" x14ac:dyDescent="0.3">
@@ -1978,7 +1978,7 @@
         <v>95</v>
       </c>
       <c r="B95" t="s">
-        <v>82</v>
+        <v>81</v>
       </c>
     </row>
     <row r="96" spans="1:2" x14ac:dyDescent="0.3">
@@ -1986,7 +1986,7 @@
         <v>96</v>
       </c>
       <c r="B96" t="s">
-        <v>83</v>
+        <v>82</v>
       </c>
     </row>
     <row r="97" spans="1:2" x14ac:dyDescent="0.3">
@@ -1994,7 +1994,7 @@
         <v>97</v>
       </c>
       <c r="B97" t="s">
-        <v>84</v>
+        <v>83</v>
       </c>
     </row>
     <row r="98" spans="1:2" x14ac:dyDescent="0.3">
@@ -2002,7 +2002,7 @@
         <v>98</v>
       </c>
       <c r="B98" t="s">
-        <v>85</v>
+        <v>84</v>
       </c>
     </row>
     <row r="99" spans="1:2" x14ac:dyDescent="0.3">
@@ -2010,7 +2010,7 @@
         <v>99</v>
       </c>
       <c r="B99" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="100" spans="1:2" x14ac:dyDescent="0.3">
@@ -2018,7 +2018,7 @@
         <v>100</v>
       </c>
       <c r="B100" t="s">
-        <v>87</v>
+        <v>86</v>
       </c>
     </row>
     <row r="101" spans="1:2" x14ac:dyDescent="0.3">
@@ -2026,7 +2026,7 @@
         <v>101</v>
       </c>
       <c r="B101" t="s">
-        <v>88</v>
+        <v>87</v>
       </c>
     </row>
     <row r="102" spans="1:2" x14ac:dyDescent="0.3">
@@ -2034,7 +2034,7 @@
         <v>102</v>
       </c>
       <c r="B102" t="s">
-        <v>89</v>
+        <v>88</v>
       </c>
     </row>
     <row r="103" spans="1:2" x14ac:dyDescent="0.3">
@@ -2042,7 +2042,7 @@
         <v>103</v>
       </c>
       <c r="B103" t="s">
-        <v>90</v>
+        <v>89</v>
       </c>
     </row>
     <row r="104" spans="1:2" x14ac:dyDescent="0.3">
@@ -2050,7 +2050,7 @@
         <v>104</v>
       </c>
       <c r="B104" t="s">
-        <v>91</v>
+        <v>90</v>
       </c>
     </row>
     <row r="105" spans="1:2" x14ac:dyDescent="0.3">
@@ -2058,7 +2058,7 @@
         <v>105</v>
       </c>
       <c r="B105" t="s">
-        <v>92</v>
+        <v>91</v>
       </c>
     </row>
     <row r="106" spans="1:2" x14ac:dyDescent="0.3">
@@ -2066,7 +2066,7 @@
         <v>106</v>
       </c>
       <c r="B106" t="s">
-        <v>93</v>
+        <v>92</v>
       </c>
     </row>
     <row r="107" spans="1:2" x14ac:dyDescent="0.3">
@@ -2074,7 +2074,7 @@
         <v>107</v>
       </c>
       <c r="B107" t="s">
-        <v>94</v>
+        <v>93</v>
       </c>
     </row>
     <row r="108" spans="1:2" x14ac:dyDescent="0.3">
@@ -2082,7 +2082,7 @@
         <v>108</v>
       </c>
       <c r="B108" t="s">
-        <v>95</v>
+        <v>94</v>
       </c>
     </row>
     <row r="109" spans="1:2" x14ac:dyDescent="0.3">
@@ -2090,7 +2090,7 @@
         <v>109</v>
       </c>
       <c r="B109" t="s">
-        <v>96</v>
+        <v>95</v>
       </c>
     </row>
     <row r="110" spans="1:2" x14ac:dyDescent="0.3">
@@ -2098,7 +2098,7 @@
         <v>110</v>
       </c>
       <c r="B110" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
     </row>
     <row r="111" spans="1:2" x14ac:dyDescent="0.3">
@@ -2106,7 +2106,7 @@
         <v>111</v>
       </c>
       <c r="B111" t="s">
-        <v>98</v>
+        <v>97</v>
       </c>
     </row>
     <row r="112" spans="1:2" x14ac:dyDescent="0.3">
@@ -2114,7 +2114,7 @@
         <v>112</v>
       </c>
       <c r="B112" t="s">
-        <v>99</v>
+        <v>98</v>
       </c>
     </row>
     <row r="113" spans="1:2" x14ac:dyDescent="0.3">
@@ -2122,7 +2122,7 @@
         <v>113</v>
       </c>
       <c r="B113" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
     </row>
     <row r="114" spans="1:2" x14ac:dyDescent="0.3">
@@ -2130,7 +2130,7 @@
         <v>114</v>
       </c>
       <c r="B114" t="s">
-        <v>101</v>
+        <v>100</v>
       </c>
     </row>
     <row r="115" spans="1:2" x14ac:dyDescent="0.3">
@@ -2138,7 +2138,7 @@
         <v>115</v>
       </c>
       <c r="B115" t="s">
-        <v>102</v>
+        <v>101</v>
       </c>
     </row>
     <row r="116" spans="1:2" x14ac:dyDescent="0.3">
@@ -2146,7 +2146,7 @@
         <v>116</v>
       </c>
       <c r="B116" t="s">
-        <v>103</v>
+        <v>102</v>
       </c>
     </row>
     <row r="117" spans="1:2" x14ac:dyDescent="0.3">
@@ -2154,7 +2154,7 @@
         <v>117</v>
       </c>
       <c r="B117" t="s">
-        <v>104</v>
+        <v>103</v>
       </c>
     </row>
     <row r="118" spans="1:2" x14ac:dyDescent="0.3">
@@ -2162,7 +2162,7 @@
         <v>118</v>
       </c>
       <c r="B118" t="s">
-        <v>105</v>
+        <v>104</v>
       </c>
     </row>
   </sheetData>

</xml_diff>